<commit_message>
a few updates to make Excel crash less. Also made CSR deductions more clear by adding a "-" sign.
</commit_message>
<xml_diff>
--- a/Excel Files/COMP_STATEMENT.xlsx
+++ b/Excel Files/COMP_STATEMENT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19920" yWindow="4530" windowWidth="25020" windowHeight="14730" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="51480" yWindow="3555" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="STATEMENT" sheetId="1" state="visible" r:id="rId1"/>
@@ -417,7 +417,7 @@
     <border>
       <left/>
       <right/>
-      <top style="hair">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -425,12 +425,41 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="hair">
         <color indexed="64"/>
       </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -449,35 +478,6 @@
         <color indexed="64"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -548,24 +548,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -574,17 +575,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -988,8 +988,8 @@
   </sheetPr>
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
@@ -1033,23 +1033,23 @@
     <row r="7" ht="4.15" customHeight="1"/>
     <row r="8" ht="4.15" customHeight="1" thickBot="1"/>
     <row r="9">
-      <c r="B9" s="22" t="inlineStr">
+      <c r="B9" s="26" t="inlineStr">
         <is>
           <t>Sales Performance</t>
         </is>
       </c>
-      <c r="C9" s="23" t="n"/>
+      <c r="C9" s="28" t="n"/>
       <c r="D9" s="3" t="n"/>
-      <c r="E9" s="22" t="inlineStr">
+      <c r="E9" s="26" t="inlineStr">
         <is>
           <t>Final Payment</t>
         </is>
       </c>
-      <c r="F9" s="38" t="n"/>
-      <c r="G9" s="23" t="n"/>
+      <c r="F9" s="27" t="n"/>
+      <c r="G9" s="28" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="32" t="inlineStr">
+      <c r="B10" s="31" t="inlineStr">
         <is>
           <t>Level 1 Sales</t>
         </is>
@@ -1058,7 +1058,7 @@
         <f>_xlfn.XLOOKUP("AM_L1_REV", payout!$G:$G, payout!$F:$F)</f>
         <v/>
       </c>
-      <c r="E10" s="32" t="inlineStr">
+      <c r="E10" s="31" t="inlineStr">
         <is>
           <t>Level 1 Payout</t>
         </is>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="11" ht="16.5" customHeight="1" thickBot="1">
       <c r="A11" s="6" t="n"/>
-      <c r="B11" s="32" t="inlineStr">
+      <c r="B11" s="31" t="inlineStr">
         <is>
           <t>Level 2 Sales</t>
         </is>
@@ -1080,7 +1080,7 @@
         <f>_xlfn.XLOOKUP("AM_L2_REV", payout!$G:$G, payout!$F:$F)</f>
         <v/>
       </c>
-      <c r="E11" s="32" t="inlineStr">
+      <c r="E11" s="31" t="inlineStr">
         <is>
           <t>Level 2 Payout</t>
         </is>
@@ -1101,51 +1101,51 @@
         <f>SUM(C10:C11)</f>
         <v/>
       </c>
-      <c r="E12" s="36" t="inlineStr">
+      <c r="E12" s="22" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="F12" s="37" t="n"/>
+      <c r="F12" s="23" t="n"/>
       <c r="G12" s="20">
         <f>SUM(G10:G11)</f>
         <v/>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1" thickTop="1">
-      <c r="E13" s="33" t="inlineStr">
+      <c r="E13" s="32" t="inlineStr">
         <is>
           <t>Other Adjustments</t>
         </is>
       </c>
-      <c r="F13" s="34" t="n"/>
+      <c r="F13" s="33" t="n"/>
       <c r="G13" s="16">
         <f>_xlfn.XLOOKUP("ADJUSTMENTS", payout!G:G,payout!F:F)</f>
         <v/>
       </c>
     </row>
-    <row r="14" hidden="1" ht="16.5" customHeight="1">
+    <row r="14" ht="16.5" customHeight="1">
       <c r="D14" s="6">
-        <f>IF(G14&gt;0, 1, 0)</f>
-        <v/>
-      </c>
-      <c r="E14" s="40" t="inlineStr">
+        <f>IF(G14&lt;0, 1, 0)</f>
+        <v/>
+      </c>
+      <c r="E14" s="30" t="inlineStr">
         <is>
           <t>CSR Deduction</t>
         </is>
       </c>
       <c r="F14" s="25" t="n"/>
       <c r="G14" s="16">
-        <f>IFERROR(_xlfn.XLOOKUP("FCE_DEDUCTION", payout!G:G,payout!F:F), 0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" hidden="1">
+        <f>IFERROR(-_xlfn.XLOOKUP("FCE_DEDUCTION", payout!G:G,payout!F:F), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
       <c r="D15" s="6">
         <f>IF(G15&gt;0, IF(G15&gt;G12, 1, 0), 0)</f>
         <v/>
       </c>
-      <c r="E15" s="35" t="inlineStr">
+      <c r="E15" s="34" t="inlineStr">
         <is>
           <t>Guarantee Adjustment</t>
         </is>
@@ -1157,36 +1157,36 @@
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E16" s="26" t="inlineStr">
+      <c r="E16" s="35" t="inlineStr">
         <is>
           <t>Net CPAS Payout</t>
         </is>
       </c>
-      <c r="F16" s="27" t="n"/>
+      <c r="F16" s="36" t="n"/>
       <c r="G16" s="8">
         <f>_xlfn.XLOOKUP("CPAS_SPIFF_PO", payout!G:G,payout!F:F)</f>
         <v/>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="E17" s="36" t="inlineStr">
+      <c r="E17" s="22" t="inlineStr">
         <is>
           <t>Final Payout</t>
         </is>
       </c>
-      <c r="F17" s="37" t="n"/>
+      <c r="F17" s="23" t="n"/>
       <c r="G17" s="9">
         <f>_xlfn.XLOOKUP("PO_AMT", payout!G:G,payout!F:F)</f>
         <v/>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="E18" s="30" t="inlineStr">
+      <c r="E18" s="37" t="inlineStr">
         <is>
           <t>YTD Payout</t>
         </is>
       </c>
-      <c r="F18" s="31" t="n"/>
+      <c r="F18" s="38" t="n"/>
       <c r="G18" s="10">
         <f>_xlfn.XLOOKUP("YTD_PO", payout!G:G,payout!F:F)</f>
         <v/>
@@ -1195,40 +1195,40 @@
     <row r="19" ht="4.15" customHeight="1"/>
     <row r="20" ht="4.15" customHeight="1"/>
     <row r="21">
-      <c r="B21" s="28" t="inlineStr">
+      <c r="B21" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Opportunity Detail </t>
         </is>
       </c>
-      <c r="C21" s="29" t="n"/>
-      <c r="D21" s="29" t="n"/>
-      <c r="E21" s="29" t="n"/>
-      <c r="F21" s="29" t="n"/>
+      <c r="C21" s="40" t="n"/>
+      <c r="D21" s="40" t="n"/>
+      <c r="E21" s="40" t="n"/>
+      <c r="F21" s="40" t="n"/>
       <c r="G21" s="25" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="39" t="inlineStr">
+      <c r="B22" s="29" t="inlineStr">
         <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="C22" s="39" t="inlineStr">
+      <c r="C22" s="29" t="inlineStr">
         <is>
           <t>Payout Type</t>
         </is>
       </c>
-      <c r="D22" s="39" t="inlineStr">
+      <c r="D22" s="29" t="inlineStr">
         <is>
           <t>Opp Name</t>
         </is>
       </c>
       <c r="E22" s="25" t="n"/>
-      <c r="F22" s="39" t="inlineStr">
+      <c r="F22" s="29" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="G22" s="39" t="inlineStr">
+      <c r="G22" s="29" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
@@ -1769,11 +1769,11 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="D40:E40"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="D27:E27"/>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1896,11 +1896,11 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>35000</v>
+        <v>41666.7</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SALES</t>
+          <t>YTD_PO</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1931,11 +1931,11 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AM_L1_REV</t>
+          <t>SALES</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AM_L2_REV</t>
+          <t>AM_L1_REV</t>
         </is>
       </c>
     </row>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2001,11 +2001,11 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AM_L1_PO</t>
+          <t>AM_L2_REV</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>AM_L2_PO</t>
+          <t>AM_L1_PO</t>
         </is>
       </c>
     </row>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2071,11 +2071,11 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>AM_TTL_PO</t>
+          <t>AM_L2_PO</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>SPIFF_DEDUCTION</t>
+          <t>AM_TTL_PO</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2141,11 +2141,11 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>CPAS_SPIFF_PO</t>
+          <t>SPIFF_DEDUCTION</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>GUR_AMT</t>
+          <t>CPAS_SPIFF_PO</t>
         </is>
       </c>
     </row>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2211,11 +2211,11 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>16666.67</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ADJUSTMENTS</t>
+          <t>GUR_AMT</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>GUR_ADJ</t>
+          <t>ADJUSTMENTS</t>
         </is>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2281,11 +2281,11 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5750</v>
+        <v>16666.67</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>PO_AMT</t>
+          <t>GUR_ADJ</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2316,11 +2316,11 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>16666.67</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>QTY</t>
+          <t>PO_AMT</t>
         </is>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2351,11 +2351,11 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>53350</v>
+        <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>YTD_PO</t>
+          <t>QTY</t>
         </is>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Joshua Gonzalez</t>
+          <t>Wade Steinhoff</t>
         </is>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jgonzalez@cvrx.com</t>
+          <t>wsteinhoff@cvrx.com</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>jheimsoth@cvrx.com</t>
+          <t>mbrown@cvrx.com</t>
         </is>
       </c>
     </row>
@@ -2425,7 +2425,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HOUSTON II (GONZALEZ)</t>
+          <t>SACRAMENTO (STEINHOFF)</t>
         </is>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2658,208 +2658,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>jgonzalez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Joshua Gonzalez</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>REP</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>SOUTH CENTRAL (HEIMSOTH)</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2024-05-20</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>MHMC 017762</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>006UY000005UgerYAC</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Memorial Hermann Memorial City Medical Center</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0010g00001mL5fJAAS</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2024_05</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Heart Failure - Reduced Ejection Fraction</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>De novo</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>35000</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>4</v>
-      </c>
-      <c r="V2" t="n">
-        <v>35000</v>
-      </c>
-      <c r="W2" t="n">
-        <v>137000</v>
-      </c>
-      <c r="X2" t="n">
-        <v>102000</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>154406.25</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>205875</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>274500</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>35000</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>Michael Mitschke</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>003UY000003Vf8SYAS</t>
-        </is>
-      </c>
-      <c r="AI2" t="n">
-        <v>5250</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>jgonzalez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Joshua Gonzalez</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>REP</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SOUTH CENTRAL (HEIMSOTH)</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2024-05-14</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>CASE# 4646</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>006UY000005NOQDYA4</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Memorial Hermann Memorial City Medical Center</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0010g00001mL5fJAAS</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2024_05</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>CPAS</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>Siddharth Mukerji</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add error handling for send_email module
</commit_message>
<xml_diff>
--- a/Excel Files/COMP_STATEMENT.xlsx
+++ b/Excel Files/COMP_STATEMENT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asorensen\PycharmProjects\comp_statements\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ABFDBE-E8E0-4AE4-8179-3EB6BEA3F04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBB2F9B-346C-4A44-A5E4-F21C8473E49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="32295" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15270" yWindow="1815" windowWidth="32295" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATEMENT" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -710,7 +709,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -737,7 +736,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,14 +761,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -781,24 +798,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1143,8 +1147,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1186,29 +1190,29 @@
     <row r="7" spans="1:7" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" ht="4.1500000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="23"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <f>_xlfn.XLOOKUP("AM_L1_REV", payout!$G:$G, payout!$F:$F)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="7">
         <f>_xlfn.XLOOKUP("AM_L1_PO", payout!G:G,payout!F:F)</f>
         <v>0</v>
@@ -1223,38 +1227,38 @@
         <f>_xlfn.XLOOKUP("AM_L2_REV", payout!$G:$G, payout!$F:$F)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="17">
+      <c r="F11" s="24"/>
+      <c r="G11" s="16">
         <f>(_xlfn.XLOOKUP("AM_L2_PO",payout!G:G,payout!F:F))</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <f>SUM(C10:C11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="20">
+      <c r="F12" s="22"/>
+      <c r="G12" s="19">
         <f>SUM(G10:G11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="16">
+      <c r="F13" s="32"/>
+      <c r="G13" s="15">
         <f>_xlfn.XLOOKUP("ADJUSTMENTS", payout!G:G,payout!F:F)</f>
         <v>0</v>
       </c>
@@ -1264,11 +1268,11 @@
         <f>IF(G14&lt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="16">
+      <c r="F14" s="24"/>
+      <c r="G14" s="15">
         <f>IFERROR(-_xlfn.XLOOKUP("FCE_DEDUCTION", payout!G:G,payout!F:F), 0)</f>
         <v>0</v>
       </c>
@@ -1278,40 +1282,40 @@
         <f>IF(G15&gt;0, IF(G15&gt;G12, 1, 0), 0)</f>
         <v>1</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="5">
         <f>IFERROR(_xlfn.XLOOKUP("GUR_AMT",payout!G:G,payout!F:F), 0)</f>
         <v>16666.669999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="27"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="8">
         <f>_xlfn.XLOOKUP("CPAS_SPIFF_PO", payout!G:G,payout!F:F)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="37"/>
+      <c r="F17" s="22"/>
       <c r="G17" s="9">
         <f>_xlfn.XLOOKUP("PO_AMT", payout!G:G,payout!F:F)</f>
         <v>16666.669999999998</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="10">
         <f>_xlfn.XLOOKUP("YTD_PO", payout!G:G,payout!F:F)</f>
         <v>58333.3</v>
@@ -1320,14 +1324,14 @@
     <row r="19" spans="2:7" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:7" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="25"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
@@ -1336,10 +1340,10 @@
       <c r="C22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="25"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
@@ -1348,530 +1352,530 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="str">
+      <c r="B23" s="40" t="str">
         <f>IF(LEN(detail!K2)&lt;1,"",detail!K2)</f>
         <v/>
       </c>
-      <c r="C23" s="12" t="str">
+      <c r="C23" s="40" t="str">
         <f>IF(LEN(detail!R2)&lt;1,"", detail!R2)</f>
         <v/>
       </c>
-      <c r="D23" s="24" t="str">
+      <c r="D23" s="23" t="str">
         <f>IF(LEN(detail!H2)&lt;1,"",detail!H2)</f>
         <v/>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="14" t="e">
+      <c r="E23" s="41"/>
+      <c r="F23" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V2)&lt;1,"",detail!V2), 0) &amp; IF(detail!W2 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G23" s="13" t="str">
+      <c r="G23" s="12" t="str">
         <f>IF(LEN(detail!T2)&lt;1,"",detail!T2)</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="str">
+      <c r="B24" s="40" t="str">
         <f>IF(LEN(detail!K3)&lt;1,"",detail!K3)</f>
         <v/>
       </c>
-      <c r="C24" s="12" t="str">
+      <c r="C24" s="40" t="str">
         <f>IF(LEN(detail!R3)&lt;1,"", detail!R3)</f>
         <v/>
       </c>
-      <c r="D24" s="24" t="str">
+      <c r="D24" s="23" t="str">
         <f>IF(LEN(detail!H3)&lt;1,"",detail!H3)</f>
         <v/>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="14" t="e">
+      <c r="E24" s="41"/>
+      <c r="F24" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V3)&lt;1,"",detail!V3), 0) &amp; IF(detail!W3 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G24" s="13" t="str">
+      <c r="G24" s="12" t="str">
         <f>IF(LEN(detail!T3)&lt;1,"",detail!T3)</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="str">
+      <c r="B25" s="40" t="str">
         <f>IF(LEN(detail!K4)&lt;1,"",detail!K4)</f>
         <v/>
       </c>
-      <c r="C25" s="12" t="str">
+      <c r="C25" s="40" t="str">
         <f>IF(LEN(detail!R4)&lt;1,"", detail!R4)</f>
         <v/>
       </c>
-      <c r="D25" s="24" t="str">
+      <c r="D25" s="23" t="str">
         <f>IF(LEN(detail!H4)&lt;1,"",detail!H4)</f>
         <v/>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="14" t="e">
+      <c r="E25" s="41"/>
+      <c r="F25" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V4)&lt;1,"",detail!V4), 0) &amp; IF(detail!W4 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G25" s="13" t="str">
+      <c r="G25" s="12" t="str">
         <f>IF(LEN(detail!T4)&lt;1,"",detail!T4)</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="str">
+      <c r="B26" s="40" t="str">
         <f>IF(LEN(detail!K5)&lt;1,"",detail!K5)</f>
         <v/>
       </c>
-      <c r="C26" s="12" t="str">
+      <c r="C26" s="40" t="str">
         <f>IF(LEN(detail!R5)&lt;1,"", detail!R5)</f>
         <v/>
       </c>
-      <c r="D26" s="24" t="str">
+      <c r="D26" s="23" t="str">
         <f>IF(LEN(detail!H5)&lt;1,"",detail!H5)</f>
         <v/>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="14" t="e">
+      <c r="E26" s="41"/>
+      <c r="F26" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V5)&lt;1,"",detail!V5), 0) &amp; IF(detail!W5 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G26" s="13" t="str">
+      <c r="G26" s="12" t="str">
         <f>IF(LEN(detail!T5)&lt;1,"",detail!T5)</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="str">
+      <c r="B27" s="40" t="str">
         <f>IF(LEN(detail!K6)&lt;1,"",detail!K6)</f>
         <v/>
       </c>
-      <c r="C27" s="12" t="str">
+      <c r="C27" s="40" t="str">
         <f>IF(LEN(detail!R6)&lt;1,"", detail!R6)</f>
         <v/>
       </c>
-      <c r="D27" s="24" t="str">
+      <c r="D27" s="23" t="str">
         <f>IF(LEN(detail!H6)&lt;1,"",detail!H6)</f>
         <v/>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="14" t="e">
+      <c r="E27" s="41"/>
+      <c r="F27" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V6)&lt;1,"",detail!V6), 0) &amp; IF(detail!W6 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G27" s="13" t="str">
+      <c r="G27" s="12" t="str">
         <f>IF(LEN(detail!T6)&lt;1,"",detail!T6)</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="12" t="str">
+      <c r="B28" s="40" t="str">
         <f>IF(LEN(detail!K7)&lt;1,"",detail!K7)</f>
         <v/>
       </c>
-      <c r="C28" s="12" t="str">
+      <c r="C28" s="40" t="str">
         <f>IF(LEN(detail!R7)&lt;1,"", detail!R7)</f>
         <v/>
       </c>
-      <c r="D28" s="24" t="str">
+      <c r="D28" s="23" t="str">
         <f>IF(LEN(detail!H7)&lt;1,"",detail!H7)</f>
         <v/>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="14" t="e">
+      <c r="E28" s="41"/>
+      <c r="F28" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V7)&lt;1,"",detail!V7), 0) &amp; IF(detail!W7 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G28" s="13" t="str">
+      <c r="G28" s="12" t="str">
         <f>IF(LEN(detail!T7)&lt;1,"",detail!T7)</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="str">
+      <c r="B29" s="40" t="str">
         <f>IF(LEN(detail!K8)&lt;1,"",detail!K8)</f>
         <v/>
       </c>
-      <c r="C29" s="12" t="str">
+      <c r="C29" s="40" t="str">
         <f>IF(LEN(detail!R8)&lt;1,"", detail!R8)</f>
         <v/>
       </c>
-      <c r="D29" s="24" t="str">
+      <c r="D29" s="23" t="str">
         <f>IF(LEN(detail!H8)&lt;1,"",detail!H8)</f>
         <v/>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="14" t="e">
+      <c r="E29" s="41"/>
+      <c r="F29" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V8)&lt;1,"",detail!V8), 0) &amp; IF(detail!W8 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G29" s="13" t="str">
+      <c r="G29" s="12" t="str">
         <f>IF(LEN(detail!T8)&lt;1,"",detail!T8)</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="str">
+      <c r="B30" s="40" t="str">
         <f>IF(LEN(detail!K9)&lt;1,"",detail!K9)</f>
         <v/>
       </c>
-      <c r="C30" s="12" t="str">
+      <c r="C30" s="40" t="str">
         <f>IF(LEN(detail!R9)&lt;1,"", detail!R9)</f>
         <v/>
       </c>
-      <c r="D30" s="24" t="str">
+      <c r="D30" s="23" t="str">
         <f>IF(LEN(detail!H9)&lt;1,"",detail!H9)</f>
         <v/>
       </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="14" t="e">
+      <c r="E30" s="41"/>
+      <c r="F30" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V9)&lt;1,"",detail!V9), 0) &amp; IF(detail!W9 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G30" s="13" t="str">
+      <c r="G30" s="12" t="str">
         <f>IF(LEN(detail!T9)&lt;1,"",detail!T9)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="str">
+      <c r="B31" s="40" t="str">
         <f>IF(LEN(detail!K10)&lt;1,"",detail!K10)</f>
         <v/>
       </c>
-      <c r="C31" s="12" t="str">
+      <c r="C31" s="40" t="str">
         <f>IF(LEN(detail!R10)&lt;1,"", detail!R10)</f>
         <v/>
       </c>
-      <c r="D31" s="24" t="str">
+      <c r="D31" s="23" t="str">
         <f>IF(LEN(detail!H10)&lt;1,"",detail!H10)</f>
         <v/>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="14" t="e">
+      <c r="E31" s="41"/>
+      <c r="F31" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V10)&lt;1,"",detail!V10), 0) &amp; IF(detail!W10 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G31" s="13" t="str">
+      <c r="G31" s="12" t="str">
         <f>IF(LEN(detail!T10)&lt;1,"",detail!T10)</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="str">
+      <c r="B32" s="40" t="str">
         <f>IF(LEN(detail!K11)&lt;1,"",detail!K11)</f>
         <v/>
       </c>
-      <c r="C32" s="12" t="str">
+      <c r="C32" s="40" t="str">
         <f>IF(LEN(detail!R11)&lt;1,"", detail!R11)</f>
         <v/>
       </c>
-      <c r="D32" s="24" t="str">
+      <c r="D32" s="23" t="str">
         <f>IF(LEN(detail!H11)&lt;1,"",detail!H11)</f>
         <v/>
       </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="14" t="e">
+      <c r="E32" s="41"/>
+      <c r="F32" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V11)&lt;1,"",detail!V11), 0) &amp; IF(detail!W11 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G32" s="13" t="str">
+      <c r="G32" s="12" t="str">
         <f>IF(LEN(detail!T11)&lt;1,"",detail!T11)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="str">
+      <c r="B33" s="40" t="str">
         <f>IF(LEN(detail!K12)&lt;1,"",detail!K12)</f>
         <v/>
       </c>
-      <c r="C33" s="12" t="str">
+      <c r="C33" s="40" t="str">
         <f>IF(LEN(detail!R12)&lt;1,"", detail!R12)</f>
         <v/>
       </c>
-      <c r="D33" s="24" t="str">
+      <c r="D33" s="23" t="str">
         <f>IF(LEN(detail!H12)&lt;1,"",detail!H12)</f>
         <v/>
       </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="14" t="e">
+      <c r="E33" s="41"/>
+      <c r="F33" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V12)&lt;1,"",detail!V12), 0) &amp; IF(detail!W12 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G33" s="13" t="str">
+      <c r="G33" s="12" t="str">
         <f>IF(LEN(detail!T12)&lt;1,"",detail!T12)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="12" t="str">
+      <c r="B34" s="40" t="str">
         <f>IF(LEN(detail!K13)&lt;1,"",detail!K13)</f>
         <v/>
       </c>
-      <c r="C34" s="12" t="str">
+      <c r="C34" s="40" t="str">
         <f>IF(LEN(detail!R13)&lt;1,"", detail!R13)</f>
         <v/>
       </c>
-      <c r="D34" s="24" t="str">
+      <c r="D34" s="23" t="str">
         <f>IF(LEN(detail!H13)&lt;1,"",detail!H13)</f>
         <v/>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="14" t="e">
+      <c r="E34" s="41"/>
+      <c r="F34" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V13)&lt;1,"",detail!V13), 0) &amp; IF(detail!W13 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G34" s="13" t="str">
+      <c r="G34" s="12" t="str">
         <f>IF(LEN(detail!T13)&lt;1,"",detail!T13)</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="str">
+      <c r="B35" s="40" t="str">
         <f>IF(LEN(detail!K14)&lt;1,"",detail!K14)</f>
         <v/>
       </c>
-      <c r="C35" s="12" t="str">
+      <c r="C35" s="40" t="str">
         <f>IF(LEN(detail!R14)&lt;1,"", detail!R14)</f>
         <v/>
       </c>
-      <c r="D35" s="24" t="str">
+      <c r="D35" s="23" t="str">
         <f>IF(LEN(detail!H14)&lt;1,"",detail!H14)</f>
         <v/>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="14" t="e">
+      <c r="E35" s="41"/>
+      <c r="F35" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V14)&lt;1,"",detail!V14), 0) &amp; IF(detail!W14 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G35" s="13" t="str">
+      <c r="G35" s="12" t="str">
         <f>IF(LEN(detail!T14)&lt;1,"",detail!T14)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="str">
+      <c r="B36" s="40" t="str">
         <f>IF(LEN(detail!K15)&lt;1,"",detail!K15)</f>
         <v/>
       </c>
-      <c r="C36" s="12" t="str">
+      <c r="C36" s="40" t="str">
         <f>IF(LEN(detail!R15)&lt;1,"", detail!R15)</f>
         <v/>
       </c>
-      <c r="D36" s="24" t="str">
+      <c r="D36" s="23" t="str">
         <f>IF(LEN(detail!H15)&lt;1,"",detail!H15)</f>
         <v/>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="14" t="e">
+      <c r="E36" s="41"/>
+      <c r="F36" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V15)&lt;1,"",detail!V15), 0) &amp; IF(detail!W15 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G36" s="13" t="str">
+      <c r="G36" s="12" t="str">
         <f>IF(LEN(detail!T15)&lt;1,"",detail!T15)</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="str">
+      <c r="B37" s="40" t="str">
         <f>IF(LEN(detail!K16)&lt;1,"",detail!K16)</f>
         <v/>
       </c>
-      <c r="C37" s="12" t="str">
+      <c r="C37" s="40" t="str">
         <f>IF(LEN(detail!R16)&lt;1,"", detail!R16)</f>
         <v/>
       </c>
-      <c r="D37" s="24" t="str">
+      <c r="D37" s="23" t="str">
         <f>IF(LEN(detail!H16)&lt;1,"",detail!H16)</f>
         <v/>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="14" t="e">
+      <c r="E37" s="41"/>
+      <c r="F37" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V16)&lt;1,"",detail!V16), 0) &amp; IF(detail!W16 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G37" s="13" t="str">
+      <c r="G37" s="12" t="str">
         <f>IF(LEN(detail!T16)&lt;1,"",detail!T16)</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="str">
+      <c r="B38" s="40" t="str">
         <f>IF(LEN(detail!K17)&lt;1,"",detail!K17)</f>
         <v/>
       </c>
-      <c r="C38" s="12" t="str">
+      <c r="C38" s="40" t="str">
         <f>IF(LEN(detail!R17)&lt;1,"", detail!R17)</f>
         <v/>
       </c>
-      <c r="D38" s="24" t="str">
+      <c r="D38" s="23" t="str">
         <f>IF(LEN(detail!H17)&lt;1,"",detail!H17)</f>
         <v/>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="14" t="e">
+      <c r="E38" s="41"/>
+      <c r="F38" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V17)&lt;1,"",detail!V17), 0) &amp; IF(detail!W17 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G38" s="13" t="str">
+      <c r="G38" s="12" t="str">
         <f>IF(LEN(detail!T17)&lt;1,"",detail!T17)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="12" t="str">
+      <c r="B39" s="40" t="str">
         <f>IF(LEN(detail!K18)&lt;1,"",detail!K18)</f>
         <v/>
       </c>
-      <c r="C39" s="12" t="str">
+      <c r="C39" s="40" t="str">
         <f>IF(LEN(detail!R18)&lt;1,"", detail!R18)</f>
         <v/>
       </c>
-      <c r="D39" s="24" t="str">
+      <c r="D39" s="23" t="str">
         <f>IF(LEN(detail!H18)&lt;1,"",detail!H18)</f>
         <v/>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="14" t="e">
+      <c r="E39" s="41"/>
+      <c r="F39" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V18)&lt;1,"",detail!V18), 0) &amp; IF(detail!W18 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G39" s="13" t="str">
+      <c r="G39" s="12" t="str">
         <f>IF(LEN(detail!T18)&lt;1,"",detail!T18)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="12" t="str">
+      <c r="B40" s="40" t="str">
         <f>IF(LEN(detail!K19)&lt;1,"",detail!K19)</f>
         <v/>
       </c>
-      <c r="C40" s="12" t="str">
+      <c r="C40" s="40" t="str">
         <f>IF(LEN(detail!R19)&lt;1,"", detail!R19)</f>
         <v/>
       </c>
-      <c r="D40" s="24" t="str">
+      <c r="D40" s="23" t="str">
         <f>IF(LEN(detail!H19)&lt;1,"",detail!H19)</f>
         <v/>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="14" t="e">
+      <c r="E40" s="41"/>
+      <c r="F40" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V19)&lt;1,"",detail!V19), 0) &amp; IF(detail!W19 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G40" s="13" t="str">
+      <c r="G40" s="12" t="str">
         <f>IF(LEN(detail!T19)&lt;1,"",detail!T19)</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="12" t="str">
+      <c r="B41" s="40" t="str">
         <f>IF(LEN(detail!K20)&lt;1,"",detail!K20)</f>
         <v/>
       </c>
-      <c r="C41" s="12" t="str">
+      <c r="C41" s="40" t="str">
         <f>IF(LEN(detail!R20)&lt;1,"", detail!R20)</f>
         <v/>
       </c>
-      <c r="D41" s="24" t="str">
+      <c r="D41" s="23" t="str">
         <f>IF(LEN(detail!H20)&lt;1,"",detail!H20)</f>
         <v/>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="14" t="e">
+      <c r="E41" s="41"/>
+      <c r="F41" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V20)&lt;1,"",detail!V20), 0) &amp; IF(detail!W20 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G41" s="13" t="str">
+      <c r="G41" s="12" t="str">
         <f>IF(LEN(detail!T20)&lt;1,"",detail!T20)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="str">
+      <c r="B42" s="40" t="str">
         <f>IF(LEN(detail!K21)&lt;1,"",detail!K21)</f>
         <v/>
       </c>
-      <c r="C42" s="12" t="str">
+      <c r="C42" s="40" t="str">
         <f>IF(LEN(detail!R21)&lt;1,"", detail!R21)</f>
         <v/>
       </c>
-      <c r="D42" s="24" t="str">
+      <c r="D42" s="23" t="str">
         <f>IF(LEN(detail!H21)&lt;1,"",detail!H21)</f>
         <v/>
       </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="14" t="e">
+      <c r="E42" s="41"/>
+      <c r="F42" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V21)&lt;1,"",detail!V21), 0) &amp; IF(detail!W21 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G42" s="13" t="str">
+      <c r="G42" s="12" t="str">
         <f>IF(LEN(detail!T21)&lt;1,"",detail!T21)</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="str">
+      <c r="B43" s="40" t="str">
         <f>IF(LEN(detail!K22)&lt;1,"",detail!K22)</f>
         <v/>
       </c>
-      <c r="C43" s="12" t="str">
+      <c r="C43" s="40" t="str">
         <f>IF(LEN(detail!R22)&lt;1,"", detail!R22)</f>
         <v/>
       </c>
-      <c r="D43" s="24" t="str">
+      <c r="D43" s="23" t="str">
         <f>IF(LEN(detail!H22)&lt;1,"",detail!H22)</f>
         <v/>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="14" t="e">
+      <c r="E43" s="41"/>
+      <c r="F43" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V22)&lt;1,"",detail!V22), 0) &amp; IF(detail!W22 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G43" s="13" t="str">
+      <c r="G43" s="12" t="str">
         <f>IF(LEN(detail!T22)&lt;1,"",detail!T22)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="str">
+      <c r="B44" s="40" t="str">
         <f>IF(LEN(detail!K23)&lt;1,"",detail!K23)</f>
         <v/>
       </c>
-      <c r="C44" s="12" t="str">
+      <c r="C44" s="40" t="str">
         <f>IF(LEN(detail!R23)&lt;1,"", detail!R23)</f>
         <v/>
       </c>
-      <c r="D44" s="24" t="str">
+      <c r="D44" s="23" t="str">
         <f>IF(LEN(detail!H23)&lt;1,"",detail!H23)</f>
         <v/>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="14" t="e">
+      <c r="E44" s="41"/>
+      <c r="F44" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V23)&lt;1,"",detail!V23), 0) &amp; IF(detail!W23 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G44" s="13" t="str">
+      <c r="G44" s="12" t="str">
         <f>IF(LEN(detail!T23)&lt;1,"",detail!T23)</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="str">
+      <c r="B45" s="40" t="str">
         <f>IF(LEN(detail!K24)&lt;1,"",detail!K24)</f>
         <v/>
       </c>
-      <c r="C45" s="12" t="str">
+      <c r="C45" s="40" t="str">
         <f>IF(LEN(detail!R24)&lt;1,"", detail!R24)</f>
         <v/>
       </c>
-      <c r="D45" s="24" t="str">
+      <c r="D45" s="23" t="str">
         <f>IF(LEN(detail!H24)&lt;1,"",detail!H24)</f>
         <v/>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="14" t="e">
+      <c r="E45" s="41"/>
+      <c r="F45" s="13" t="e">
         <f>DOLLAR(IF(LEN(detail!V24)&lt;1,"",detail!V24), 0) &amp; IF(detail!W24 = 1, "*", "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G45" s="13" t="str">
+      <c r="G45" s="12" t="str">
         <f>IF(LEN(detail!T24)&lt;1,"",detail!T24)</f>
         <v/>
       </c>
@@ -1883,26 +1887,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D40:E40"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D25:E25"/>
@@ -1918,7 +1902,27 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:D45 F23:G45">
     <cfRule type="containsErrors" dxfId="0" priority="1">
@@ -1940,28 +1944,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2349,115 +2353,115 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="X1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="Y1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="Z1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AA1" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AC1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AD1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AE1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AF1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AG1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AI1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AK1" s="20" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>